<commit_message>
premier done , bundesliga half done
</commit_message>
<xml_diff>
--- a/premier/premier_updated.xlsx
+++ b/premier/premier_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\scraping-fbref\premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC4F33B-DEDB-4352-9CDD-42F4CBEE15E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C2C941-D50A-4DCD-93D1-A4C37EBC8019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,6 +578,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -925,7 +926,7 @@
   <dimension ref="A1:AE381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>